<commit_message>
fix: matsmo variable units and labels
</commit_message>
<xml_diff>
--- a/dictionaries/outcome/1_5/1_5_yearly_rep.xlsx
+++ b/dictionaries/outcome/1_5/1_5_yearly_rep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sidohaakma/Documents/Development/Source/Visual/ds-dictionaries/dictionaries/outcome/1_5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD552F2-2506-A24F-98D6-BD3EB00F4448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{874D7CC3-C81A-4047-9904-361BFA01AEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33600" yWindow="-6600" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1136,9 +1136,6 @@
     <t>inh_all_sens_SPT_TREE_mix_</t>
   </si>
   <si>
-    <t>Calculated smoking score using DNAsmokeR</t>
-  </si>
-  <si>
     <t>Type of DNA methylation array used to create smoking score</t>
   </si>
   <si>
@@ -1212,6 +1209,9 @@
   </si>
   <si>
     <t>matsmo_age_at_dna_methyl_</t>
+  </si>
+  <si>
+    <t>Calculated smoking score using DNAsmokeR (value ranging between 0 to 1)</t>
   </si>
 </sst>
 </file>
@@ -1848,8 +1848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG139"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A125" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C141" sqref="C141"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A119" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3785,21 +3785,21 @@
     </row>
     <row r="134" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>393</v>
-      </c>
-      <c r="B134" t="s">
-        <v>5</v>
+        <v>392</v>
+      </c>
+      <c r="B134" s="24" t="s">
+        <v>12</v>
       </c>
       <c r="C134" t="s">
-        <v>12</v>
-      </c>
-      <c r="D134" t="s">
-        <v>369</v>
+        <v>6</v>
+      </c>
+      <c r="D134" s="18" t="s">
+        <v>394</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B135" t="s">
         <v>5</v>
@@ -3808,26 +3808,26 @@
         <v>6</v>
       </c>
       <c r="D135" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>394</v>
-      </c>
-      <c r="B136" t="s">
-        <v>5</v>
+        <v>393</v>
+      </c>
+      <c r="B136" s="24" t="s">
+        <v>12</v>
       </c>
       <c r="C136" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D136" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B137" t="s">
         <v>5</v>
@@ -3836,12 +3836,12 @@
         <v>6</v>
       </c>
       <c r="D137" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B138" t="s">
         <v>5</v>
@@ -3850,12 +3850,12 @@
         <v>6</v>
       </c>
       <c r="D138" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="25" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B139" s="24" t="s">
         <v>12</v>
@@ -3864,7 +3864,7 @@
         <v>17</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>
@@ -7310,7 +7310,7 @@
     </row>
     <row r="245" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A245" s="22" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B245" s="23">
         <v>1</v>
@@ -7319,12 +7319,12 @@
         <v>0</v>
       </c>
       <c r="D245" s="23" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="246" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A246" s="22" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B246" s="23">
         <v>2</v>
@@ -7333,12 +7333,12 @@
         <v>0</v>
       </c>
       <c r="D246" s="23" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="247" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A247" s="22" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B247" s="23">
         <v>1</v>
@@ -7347,12 +7347,12 @@
         <v>0</v>
       </c>
       <c r="D247" s="23" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="248" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A248" s="22" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B248" s="23">
         <v>2</v>
@@ -7361,12 +7361,12 @@
         <v>0</v>
       </c>
       <c r="D248" s="23" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="249" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A249" s="22" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B249" s="23">
         <v>3</v>
@@ -7375,26 +7375,26 @@
         <v>0</v>
       </c>
       <c r="D249" s="23" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="250" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A250" s="22" t="s">
+        <v>380</v>
+      </c>
+      <c r="B250" s="23">
+        <v>0</v>
+      </c>
+      <c r="C250" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D250" s="23" t="s">
         <v>381</v>
-      </c>
-      <c r="B250" s="23">
-        <v>0</v>
-      </c>
-      <c r="C250" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="D250" s="23" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="251" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A251" s="22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B251" s="23">
         <v>1</v>
@@ -7403,12 +7403,12 @@
         <v>0</v>
       </c>
       <c r="D251" s="23" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="252" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A252" s="22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B252" s="23">
         <v>2</v>
@@ -7417,12 +7417,12 @@
         <v>0</v>
       </c>
       <c r="D252" s="23" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="253" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A253" s="22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B253" s="23">
         <v>3</v>
@@ -7436,7 +7436,7 @@
     </row>
     <row r="254" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A254" s="22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B254" s="23">
         <v>4</v>
@@ -7445,12 +7445,12 @@
         <v>0</v>
       </c>
       <c r="D254" s="23" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="255" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A255" s="22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B255" s="23">
         <v>5</v>
@@ -7459,12 +7459,12 @@
         <v>0</v>
       </c>
       <c r="D255" s="23" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="256" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A256" s="22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B256" s="23">
         <v>6</v>
@@ -7473,12 +7473,12 @@
         <v>0</v>
       </c>
       <c r="D256" s="23" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="257" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A257" s="22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B257" s="23">
         <v>7</v>
@@ -7487,12 +7487,12 @@
         <v>0</v>
       </c>
       <c r="D257" s="23" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="258" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A258" s="22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B258" s="23">
         <v>8</v>
@@ -7501,12 +7501,12 @@
         <v>0</v>
       </c>
       <c r="D258" s="23" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="259" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A259" s="22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B259" s="23">
         <v>9</v>
@@ -7515,7 +7515,7 @@
         <v>0</v>
       </c>
       <c r="D259" s="23" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>